<commit_message>
Added daily high, low, dividend tracking and implemented dividend reinvestment
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -28,22 +28,28 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="0.8917in"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="0.889in"/>
+    </style:style>
+    <style:style style:name="co3" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.9311in"/>
     </style:style>
-    <style:style style:name="co3" style:family="table-column">
+    <style:style style:name="co4" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.9862in"/>
     </style:style>
-    <style:style style:name="co4" style:family="table-column">
+    <style:style style:name="co5" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.7508in"/>
     </style:style>
-    <style:style style:name="co5" style:family="table-column">
+    <style:style style:name="co6" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="2.1811in"/>
     </style:style>
-    <style:style style:name="co6" style:family="table-column">
+    <style:style style:name="co7" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.611in"/>
     </style:style>
-    <style:style style:name="co7" style:family="table-column">
+    <style:style style:name="co8" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.472in"/>
+    </style:style>
+    <style:style style:name="co9" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.0146in"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.1917in" fo:break-before="auto" style:use-optimal-row-height="false"/>
@@ -87,22 +93,22 @@
       <number:number number:decimal-places="2" loext:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N104P0"/>
     </number:currency-style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
-    </style:style>
     <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
     <style:style style:name="ce24" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
+      <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
+    </style:style>
+    <style:style style:name="ce12" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
+      <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
+      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Calibri" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
+    </style:style>
+    <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
@@ -208,42 +214,42 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce23" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Today's change</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce24" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
             <text:p>Total cost</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce24" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
             <text:p>Total market value</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce24" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
             <text:p>Total gain/loss</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce24" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
             <text:p>Total gain/loss (%)</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce23"/>
+          <table:table-cell table:style-name="ce12"/>
           <table:table-cell table:number-columns-repeated="62"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -252,14 +258,16 @@
       </table:table>
       <table:table table:name="Current" table:style-name="ta2">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="ce24"/>
-        <table:table-column table:style-name="co3" table:number-columns-repeated="2" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co4" table:number-columns-repeated="2" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co5" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co4" table:number-columns-repeated="2" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co7" table:default-cell-style-name="ce23"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="54" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="ce21"/>
+        <table:table-column table:style-name="co4" table:number-columns-repeated="2" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co5" table:number-columns-repeated="2" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co7" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co5" table:number-columns-repeated="2" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co8" table:default-cell-style-name="ce12"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="4" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co9" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="49" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Investment Name</text:p>
@@ -291,14 +299,23 @@
           <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Gain/Loss (%)</text:p>
           </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>High</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>Low</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>Dividends</text:p>
+          </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce23" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Today’s change</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce20" office:value-type="currency" office:currency="USD" office:value="0" calcext:value-type="currency">
             <text:p>$0.00</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="51"/>
+          <table:table-cell table:number-columns-repeated="48"/>
         </table:table-row>
         <table:table-row-group>
           <table:table-row table:style-name="ro1">
@@ -332,14 +349,14 @@
             <table:table-cell table:style-name="ce19" office:value-type="float" office:value="17.8502626845419" calcext:value-type="float">
               <text:p>17.8502626845419</text:p>
             </table:table-cell>
-            <table:table-cell/>
-            <table:table-cell table:style-name="ce23" office:value-type="string" calcext:value-type="string">
+            <table:table-cell table:number-columns-repeated="4"/>
+            <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
               <text:p>Prior day’s portfolio value</text:p>
             </table:table-cell>
             <table:table-cell table:style-name="ce42" office:value-type="float" office:value="0" calcext:value-type="float">
               <text:p>0</text:p>
             </table:table-cell>
-            <table:table-cell table:number-columns-repeated="51"/>
+            <table:table-cell table:number-columns-repeated="48"/>
           </table:table-row>
           <table:table-row table:style-name="ro1">
             <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -507,11 +524,11 @@
     <meta:initial-creator>Flynn-Elhoffer, Scott</meta:initial-creator>
     <dc:language>en-US</dc:language>
     <meta:creation-date>2020-03-30T17:52:20</meta:creation-date>
-    <dc:date>2020-09-19T00:27:13.472170100</dc:date>
-    <meta:editing-cycles>23</meta:editing-cycles>
+    <dc:date>2020-09-26T18:16:33.171438358</dc:date>
+    <meta:editing-cycles>24</meta:editing-cycles>
     <meta:generator>LibreOffice/6.4.5.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
-    <meta:editing-duration>PT3M45S</meta:editing-duration>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="75" meta:object-count="0"/>
+    <meta:editing-duration>PT4M57S</meta:editing-duration>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="78" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">3.0</meta:user-defined>
   </office:meta>
 </office:document-meta>
@@ -523,21 +540,21 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">55488</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">65135</config:config-item>
       <config:config-item config:name="VisibleAreaHeight" config:type="int">3868</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Current">
-              <config:config-item config:name="CursorPositionX" config:type="int">11</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
               <config:config-item config:name="VerticalSplitPosition" config:type="int">0</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">4</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
@@ -567,7 +584,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Current</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1469</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">965</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -604,7 +621,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">vgH+/1NhbXN1bmdfWDc2MDBfU2VyaWVzX1NFQzg0MjUxOTEyNzZCMl9teG9fc19NYWNCb29rX1BybwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpTYW1zdW5nX1g3NjAwX1Nlcmllc19TRUM4NAAWAAMA3wAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9U2Ftc3VuZ19YNzYwMF9TZXJpZXNfU0VDODQyNTE5MTI3NkIyX214b19zX01hY0Jvb2tfUHJvCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpMZXR0ZXIAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAuAAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpMZXR0ZXIAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">2</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -617,7 +634,7 @@
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">Samsung_X7600_Series_SEC8425191276B2_mxo_s_MacBook_Pro</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
@@ -1047,9 +1064,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2020-09-19">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2020-09-26">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="00:23:28.255493193">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="18:15:20.823911606">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>